<commit_message>
Update Shadow Rate with Latest Data
</commit_message>
<xml_diff>
--- a/exhibits/shadowrate.xlsx
+++ b/exhibits/shadowrate.xlsx
@@ -13,7 +13,187 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fedfundsrate</t>
+  </si>
+  <si>
+    <t>fedfundsrate_shadow</t>
+  </si>
   <si>
     <t>date</t>
   </si>
@@ -51,7 +231,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -61,14 +241,54 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -78,7 +298,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C150"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="true"/>
@@ -88,13 +308,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2">
@@ -102,10 +322,10 @@
         <v>1984</v>
       </c>
       <c r="B2" s="0">
-        <v>9.6866666666667545</v>
+        <v>9.6866666666665768</v>
       </c>
       <c r="C2" s="0">
-        <v>9.6866666666667545</v>
+        <v>9.6866666666665768</v>
       </c>
     </row>
     <row r="3">
@@ -116,7 +336,7 @@
         <v>10.556666666666658</v>
       </c>
       <c r="C3" s="0">
-        <v>10.556666666666747</v>
+        <v>10.556666666666569</v>
       </c>
     </row>
     <row r="4">
@@ -127,7 +347,7 @@
         <v>11.38999999999999</v>
       </c>
       <c r="C4" s="0">
-        <v>11.390000000000079</v>
+        <v>11.389999999999878</v>
       </c>
     </row>
     <row r="5">
@@ -138,7 +358,7 @@
         <v>9.2666666666667119</v>
       </c>
       <c r="C5" s="0">
-        <v>9.2666666666668007</v>
+        <v>9.2666666666666231</v>
       </c>
     </row>
     <row r="6">
@@ -149,7 +369,7 @@
         <v>8.4766666666667092</v>
       </c>
       <c r="C6" s="0">
-        <v>8.476666666666798</v>
+        <v>8.4766666666667092</v>
       </c>
     </row>
     <row r="7">
@@ -160,7 +380,7 @@
         <v>7.9233333333333045</v>
       </c>
       <c r="C7" s="0">
-        <v>7.9233333333333933</v>
+        <v>7.9233333333333045</v>
       </c>
     </row>
     <row r="8">
@@ -171,7 +391,7 @@
         <v>7.9000000000000181</v>
       </c>
       <c r="C8" s="0">
-        <v>7.9000000000001069</v>
+        <v>7.9000000000000181</v>
       </c>
     </row>
     <row r="9">
@@ -182,7 +402,7 @@
         <v>8.1033333333333513</v>
       </c>
       <c r="C9" s="0">
-        <v>8.1033333333334401</v>
+        <v>8.1033333333333513</v>
       </c>
     </row>
     <row r="10">
@@ -193,7 +413,7 @@
         <v>7.8266666666666485</v>
       </c>
       <c r="C10" s="0">
-        <v>7.8266666666667373</v>
+        <v>7.8266666666665596</v>
       </c>
     </row>
     <row r="11">
@@ -204,7 +424,7 @@
         <v>6.9199999999999484</v>
       </c>
       <c r="C11" s="0">
-        <v>6.9200000000000372</v>
+        <v>6.9199999999998596</v>
       </c>
     </row>
     <row r="12">
@@ -215,7 +435,7 @@
         <v>6.2066666666666936</v>
       </c>
       <c r="C12" s="0">
-        <v>6.2066666666667825</v>
+        <v>6.2066666666666048</v>
       </c>
     </row>
     <row r="13">
@@ -226,7 +446,7 @@
         <v>6.266666666666687</v>
       </c>
       <c r="C13" s="0">
-        <v>6.2666666666667759</v>
+        <v>6.266666666666687</v>
       </c>
     </row>
     <row r="14">
@@ -237,7 +457,7 @@
         <v>6.2200000000000033</v>
       </c>
       <c r="C14" s="0">
-        <v>6.2200000000000921</v>
+        <v>6.2200000000000033</v>
       </c>
     </row>
     <row r="15">
@@ -248,7 +468,7 @@
         <v>6.6499999999999782</v>
       </c>
       <c r="C15" s="0">
-        <v>6.650000000000067</v>
+        <v>6.6499999999999782</v>
       </c>
     </row>
     <row r="16">
@@ -259,7 +479,7 @@
         <v>6.843333333333379</v>
       </c>
       <c r="C16" s="0">
-        <v>6.8433333333334678</v>
+        <v>6.843333333333379</v>
       </c>
     </row>
     <row r="17">
@@ -270,7 +490,7 @@
         <v>6.9166666666666377</v>
       </c>
       <c r="C17" s="0">
-        <v>6.9166666666667265</v>
+        <v>6.9166666666666377</v>
       </c>
     </row>
     <row r="18">
@@ -281,7 +501,7 @@
         <v>6.6633333333333544</v>
       </c>
       <c r="C18" s="0">
-        <v>6.6633333333334432</v>
+        <v>6.6633333333333544</v>
       </c>
     </row>
     <row r="19">
@@ -292,7 +512,7 @@
         <v>7.1566666666666556</v>
       </c>
       <c r="C19" s="0">
-        <v>7.1566666666667667</v>
+        <v>7.1566666666666556</v>
       </c>
     </row>
     <row r="20">
@@ -314,7 +534,7 @@
         <v>8.470000000000022</v>
       </c>
       <c r="C21" s="0">
-        <v>8.470000000000022</v>
+        <v>8.4699999999999331</v>
       </c>
     </row>
     <row r="22">
@@ -325,7 +545,7 @@
         <v>9.4433333333333813</v>
       </c>
       <c r="C22" s="0">
-        <v>9.4433333333333813</v>
+        <v>9.4433333333332925</v>
       </c>
     </row>
     <row r="23">
@@ -336,7 +556,7 @@
         <v>9.7266666666666612</v>
       </c>
       <c r="C23" s="0">
-        <v>9.7266666666666612</v>
+        <v>9.7266666666665724</v>
       </c>
     </row>
     <row r="24">
@@ -347,7 +567,7 @@
         <v>9.0833333333332877</v>
       </c>
       <c r="C24" s="0">
-        <v>9.0833333333332877</v>
+        <v>9.0833333333331989</v>
       </c>
     </row>
     <row r="25">
@@ -358,7 +578,7 @@
         <v>8.6133333333333404</v>
       </c>
       <c r="C25" s="0">
-        <v>8.6133333333333404</v>
+        <v>8.6133333333332516</v>
       </c>
     </row>
     <row r="26">
@@ -369,7 +589,7 @@
         <v>8.2500000000000462</v>
       </c>
       <c r="C26" s="0">
-        <v>8.2500000000000462</v>
+        <v>8.2499999999999574</v>
       </c>
     </row>
     <row r="27">
@@ -413,7 +633,7 @@
         <v>6.4266666666667138</v>
       </c>
       <c r="C30" s="0">
-        <v>6.4266666666667138</v>
+        <v>6.426666666666625</v>
       </c>
     </row>
     <row r="31">
@@ -919,7 +1139,7 @@
         <v>1.7400000000000304</v>
       </c>
       <c r="C76" s="0">
-        <v>1.739982825893116</v>
+        <v>1.7400000000000304</v>
       </c>
     </row>
     <row r="77">
@@ -930,7 +1150,7 @@
         <v>1.4433333333333298</v>
       </c>
       <c r="C77" s="0">
-        <v>1.4433315379358103</v>
+        <v>1.4433333333333298</v>
       </c>
     </row>
     <row r="78">
@@ -941,7 +1161,7 @@
         <v>1.2499999999999956</v>
       </c>
       <c r="C78" s="0">
-        <v>1.25003023433925</v>
+        <v>1.2499999999999956</v>
       </c>
     </row>
     <row r="79">
@@ -952,7 +1172,7 @@
         <v>1.246666666666707</v>
       </c>
       <c r="C79" s="0">
-        <v>1.2467387340013181</v>
+        <v>1.246666666666707</v>
       </c>
     </row>
     <row r="80">
@@ -963,7 +1183,7 @@
         <v>1.0166666666666879</v>
       </c>
       <c r="C80" s="0">
-        <v>1.0167849788565775</v>
+        <v>1.0166666666666879</v>
       </c>
     </row>
     <row r="81">
@@ -974,7 +1194,7 @@
         <v>0.99666666666664572</v>
       </c>
       <c r="C81" s="0">
-        <v>0.99683172923572538</v>
+        <v>0.99638312099048498</v>
       </c>
     </row>
     <row r="82">
@@ -985,7 +1205,7 @@
         <v>1.0033333333333116</v>
       </c>
       <c r="C82" s="0">
-        <v>1.0035422769654412</v>
+        <v>1.0029047998475038</v>
       </c>
     </row>
     <row r="83">
@@ -996,7 +1216,7 @@
         <v>1.0099999999999998</v>
       </c>
       <c r="C83" s="0">
-        <v>1.0102474462577282</v>
+        <v>1.0095083296175922</v>
       </c>
     </row>
     <row r="84">
@@ -1007,7 +1227,7 @@
         <v>1.4333333333332865</v>
       </c>
       <c r="C84" s="0">
-        <v>1.4336129935576203</v>
+        <v>1.4328298615421842</v>
       </c>
     </row>
     <row r="85">
@@ -1018,7 +1238,7 @@
         <v>1.9500000000000517</v>
       </c>
       <c r="C85" s="0">
-        <v>1.9503038988276877</v>
+        <v>1.949519841192604</v>
       </c>
     </row>
     <row r="86">
@@ -1029,7 +1249,7 @@
         <v>2.46999999999995</v>
       </c>
       <c r="C86" s="0">
-        <v>2.4703192092139448</v>
+        <v>2.4695666422738238</v>
       </c>
     </row>
     <row r="87">
@@ -1040,7 +1260,7 @@
         <v>2.9433333333333422</v>
       </c>
       <c r="C87" s="0">
-        <v>2.9436584032227264</v>
+        <v>2.9429614988056185</v>
       </c>
     </row>
     <row r="88">
@@ -1051,7 +1271,7 @@
         <v>3.4600000000000408</v>
       </c>
       <c r="C88" s="0">
-        <v>3.4603215999805759</v>
+        <v>3.4596973846305001</v>
       </c>
     </row>
     <row r="89">
@@ -1062,7 +1282,7 @@
         <v>3.980000000000028</v>
       </c>
       <c r="C89" s="0">
-        <v>3.980308852765635</v>
+        <v>3.9797693220471109</v>
       </c>
     </row>
     <row r="90">
@@ -1073,7 +1293,7 @@
         <v>4.4566666666666865</v>
       </c>
       <c r="C90" s="0">
-        <v>4.4569537310657159</v>
+        <v>4.4565068918595463</v>
       </c>
     </row>
     <row r="91">
@@ -1084,7 +1304,7 @@
         <v>4.9066666666667036</v>
       </c>
       <c r="C91" s="0">
-        <v>4.9069234355365143</v>
+        <v>4.9065739074908077</v>
       </c>
     </row>
     <row r="92">
@@ -1095,7 +1315,7 @@
         <v>5.2466666666666884</v>
       </c>
       <c r="C92" s="0">
-        <v>5.2468851089322088</v>
+        <v>5.2466350660383743</v>
       </c>
     </row>
     <row r="93">
@@ -1106,7 +1326,7 @@
         <v>5.2466666666666884</v>
       </c>
       <c r="C93" s="0">
-        <v>5.2468392337918779</v>
+        <v>5.2466889058359056</v>
       </c>
     </row>
     <row r="94">
@@ -1117,7 +1337,7 @@
         <v>5.2566666666666872</v>
       </c>
       <c r="C94" s="0">
-        <v>5.2567872035203189</v>
+        <v>5.2567344970156249</v>
       </c>
     </row>
     <row r="95">
@@ -1128,7 +1348,7 @@
         <v>5.2499999999999547</v>
       </c>
       <c r="C95" s="0">
-        <v>5.2500631002248221</v>
+        <v>5.2501048540359641</v>
       </c>
     </row>
     <row r="96">
@@ -1139,7 +1359,7 @@
         <v>5.0733333333333519</v>
       </c>
       <c r="C96" s="0">
-        <v>5.0733343788116558</v>
+        <v>5.073466484556155</v>
       </c>
     </row>
     <row r="97">
@@ -1150,7 +1370,7 @@
         <v>4.4966666666666821</v>
       </c>
       <c r="C97" s="0">
-        <v>4.4966021364661657</v>
+        <v>4.4968192910172844</v>
       </c>
     </row>
     <row r="98">
@@ -1161,7 +1381,7 @@
         <v>3.1766666666666721</v>
       </c>
       <c r="C98" s="0">
-        <v>3.1765346965513697</v>
+        <v>3.1768298489961877</v>
       </c>
     </row>
     <row r="99">
@@ -1172,7 +1392,7 @@
         <v>2.0866666666666589</v>
       </c>
       <c r="C99" s="0">
-        <v>2.0864658243070711</v>
+        <v>2.0868331992731415</v>
       </c>
     </row>
     <row r="100">
@@ -1183,7 +1403,7 @@
         <v>1.9400000000000306</v>
       </c>
       <c r="C100" s="0">
-        <v>1.9397277569163318</v>
+        <v>1.9401643070454666</v>
       </c>
     </row>
     <row r="101">
@@ -1194,7 +1414,7 @@
         <v>0.50666666666669968</v>
       </c>
       <c r="C101" s="0">
-        <v>0.50664727500135953</v>
+        <v>0.50777465922533516</v>
       </c>
     </row>
     <row r="102">
@@ -1205,7 +1425,7 @@
         <v>0</v>
       </c>
       <c r="C102" s="0">
-        <v>1.2672168426830943</v>
+        <v>1.6488952284639868</v>
       </c>
     </row>
     <row r="103">
@@ -1216,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="0">
-        <v>0.35974063543589008</v>
+        <v>0.62422887211277533</v>
       </c>
     </row>
     <row r="104">
@@ -1227,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="0">
-        <v>-0.25618758611023473</v>
+        <v>-0.11067726072560014</v>
       </c>
     </row>
     <row r="105">
@@ -1238,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="0">
-        <v>-0.27518257468277518</v>
+        <v>-0.16189799346500999</v>
       </c>
     </row>
     <row r="106">
@@ -1249,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="0">
-        <v>-0.14322134107797035</v>
+        <v>-0.12751431539200775</v>
       </c>
     </row>
     <row r="107">
@@ -1260,7 +1480,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="0">
-        <v>-0.96390615330738116</v>
+        <v>-1.1848463498480011</v>
       </c>
     </row>
     <row r="108">
@@ -1271,7 +1491,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="0">
-        <v>-1.0885926994627759</v>
+        <v>-1.0859586593229498</v>
       </c>
     </row>
     <row r="109">
@@ -1282,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="0">
-        <v>-1.5031596898349875</v>
+        <v>-1.5402196670599944</v>
       </c>
     </row>
     <row r="110">
@@ -1293,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="0">
-        <v>-1.5144960632580862</v>
+        <v>-1.3623043248304323</v>
       </c>
     </row>
     <row r="111">
@@ -1304,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="0">
-        <v>-1.0962839897474486</v>
+        <v>-1.0891450601857144</v>
       </c>
     </row>
     <row r="112">
@@ -1315,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="0">
-        <v>-1.722725403314207</v>
+        <v>-1.8674739911055394</v>
       </c>
     </row>
     <row r="113">
@@ -1326,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="C113" s="0">
-        <v>-1.1252827949940314</v>
+        <v>-1.2162518929261901</v>
       </c>
     </row>
     <row r="114">
@@ -1337,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="C114" s="0">
-        <v>-2.0106295454326073</v>
+        <v>-2.009660476457209</v>
       </c>
     </row>
     <row r="115">
@@ -1348,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="0">
-        <v>-1.850651502057421</v>
+        <v>-1.6607243994285259</v>
       </c>
     </row>
     <row r="116">
@@ -1359,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="C116" s="0">
-        <v>-1.4770730817615485</v>
+        <v>-1.2895588468961661</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1590,7 @@
         <v>0</v>
       </c>
       <c r="C117" s="0">
-        <v>-2.6820440919218647</v>
+        <v>-2.4213785264856846</v>
       </c>
     </row>
     <row r="118">
@@ -1381,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="C118" s="0">
-        <v>-1.4549628214281962</v>
+        <v>-1.1357874445460658</v>
       </c>
     </row>
     <row r="119">
@@ -1392,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="C119" s="0">
-        <v>-0.85972867189337832</v>
+        <v>-0.63276879257986307</v>
       </c>
     </row>
     <row r="120">
@@ -1403,7 +1623,7 @@
         <v>0</v>
       </c>
       <c r="C120" s="0">
-        <v>-0.55580511273184419</v>
+        <v>-0.45619773641784045</v>
       </c>
     </row>
     <row r="121">
@@ -1414,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="C121" s="0">
-        <v>-0.63122979831121695</v>
+        <v>-0.54336708914966003</v>
       </c>
     </row>
     <row r="122">
@@ -1425,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="C122" s="0">
-        <v>-0.86572208981484655</v>
+        <v>-0.74278953819548743</v>
       </c>
     </row>
     <row r="123">
@@ -1436,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="C123" s="0">
-        <v>-0.7961773641566805</v>
+        <v>-0.72762278155045212</v>
       </c>
     </row>
     <row r="124">
@@ -1447,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="C124" s="0">
-        <v>-0.5631450152898454</v>
+        <v>-0.4624926551333397</v>
       </c>
     </row>
     <row r="125">
@@ -1458,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="C125" s="0">
-        <v>-0.32280313536572347</v>
+        <v>-0.21961124805635057</v>
       </c>
     </row>
     <row r="126">
@@ -1469,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="C126" s="0">
-        <v>-0.083958571131270698</v>
+        <v>0.16225716019162562</v>
       </c>
     </row>
     <row r="127">
@@ -1480,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="C127" s="0">
-        <v>0.010653991576758948</v>
+        <v>0.032963145757958223</v>
       </c>
     </row>
     <row r="128">
@@ -1491,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="C128" s="0">
-        <v>-0.00048591886001592144</v>
+        <v>0.05031697791864076</v>
       </c>
     </row>
     <row r="129">
@@ -1681,6 +1901,61 @@
         <v>1.6433333333332856</v>
       </c>
     </row>
+    <row r="146">
+      <c r="A146" s="0">
+        <v>2020</v>
+      </c>
+      <c r="B146" s="0">
+        <v>1.2599999999999723</v>
+      </c>
+      <c r="C146" s="0">
+        <v>1.2599999999999723</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0">
+        <v>2020.25</v>
+      </c>
+      <c r="B147" s="0">
+        <v>0</v>
+      </c>
+      <c r="C147" s="0">
+        <v>7.6631433313967046</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0">
+        <v>2020.5</v>
+      </c>
+      <c r="B148" s="0">
+        <v>0</v>
+      </c>
+      <c r="C148" s="0">
+        <v>-4.7850751537857779</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0">
+        <v>2020.75</v>
+      </c>
+      <c r="B149" s="0">
+        <v>0</v>
+      </c>
+      <c r="C149" s="0">
+        <v>-3.048671875166753</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0">
+        <v>2021</v>
+      </c>
+      <c r="B150" s="0">
+        <v>0</v>
+      </c>
+      <c r="C150" s="0">
+        <v>-3.4569946319478295</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>